<commit_message>
added acceptable answers to cancer screening
</commit_message>
<xml_diff>
--- a/Data/Test_Question_File.3_15.xlsx
+++ b/Data/Test_Question_File.3_15.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://huroncg-my.sharepoint.com/personal/johsnyder_huronconsultinggroup_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://huroncg-my.sharepoint.com/personal/khirst_huronconsultinggroup_com/Documents/Desktop/RPA/VA Project/ML_RPA_Use_Cases/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{A196FC46-37C7-497A-8168-3DF98752043B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EA1CA1D-A707-4164-B211-3B31D850538E}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="8_{A196FC46-37C7-497A-8168-3DF98752043B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F22F89CC-F6B1-4F35-822A-D32B41D5562C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A809188-EDBE-4730-9950-7A0D0331F8B9}"/>
+    <workbookView xWindow="-20970" yWindow="9345" windowWidth="17130" windowHeight="14625" xr2:uid="{3A809188-EDBE-4730-9950-7A0D0331F8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Cancer" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Code</t>
   </si>
@@ -68,27 +68,18 @@
     <t>Do You Get Income From Social Security?</t>
   </si>
   <si>
-    <t>Yes;No</t>
-  </si>
-  <si>
     <t>KIQ005</t>
   </si>
   <si>
     <t>How Often Do You Have Urinary Leakage per week?</t>
   </si>
   <si>
-    <t>Once;Twice;Thrice</t>
-  </si>
-  <si>
     <t>AUQ054</t>
   </si>
   <si>
     <t>General Condition of Hearing?</t>
   </si>
   <si>
-    <t>Great;Good;Average;Poor</t>
-  </si>
-  <si>
     <t>MCQ560</t>
   </si>
   <si>
@@ -113,9 +104,6 @@
     <t>Main Reason for Visiting Dentist?</t>
   </si>
   <si>
-    <t>Checkup;Surgery;Cavity</t>
-  </si>
-  <si>
     <t>MCQ092</t>
   </si>
   <si>
@@ -138,6 +126,21 @@
   </si>
   <si>
     <t xml:space="preserve">Any Chemical Products Used to Kill Weeds? </t>
+  </si>
+  <si>
+    <t>Yes;No;Refused;Don't Know;Missing</t>
+  </si>
+  <si>
+    <t>Never;Less than once a month;A few times a month;A few times a week; Ever day and/or night; Refused;Don't Know;Missing</t>
+  </si>
+  <si>
+    <t>Excellent;Good;A little trouble;Moderate hearing trouble;A lot of trouble;Deaf;Refused;Don't Know;Missing</t>
+  </si>
+  <si>
+    <t>Went in on own for check-up, examination, or cleaning;Was called in by dentist for check-up, examination, or cleaning;Something was wrong, bothering, or hurting; Went for treatment of a condition that dentist previously discovered;Other;Refused;Don't Know;Missing</t>
+  </si>
+  <si>
+    <t>Not at all;Several Days;More than half the days;Nearly every day;Refused;Don't Know;Missing</t>
   </si>
 </sst>
 </file>
@@ -217,10 +220,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,18 +535,18 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="234.31640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -569,117 +568,117 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="C12" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -697,7 +696,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
crosswalk added for cancer questions. bot reads all inputs, reads each question sheet specific to the condition selected, finds the coefficient for answer provided and writes coefficient in test question file
</commit_message>
<xml_diff>
--- a/Data/Test_Question_File.3_15.xlsx
+++ b/Data/Test_Question_File.3_15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://huroncg-my.sharepoint.com/personal/khirst_huronconsultinggroup_com/Documents/Desktop/RPA/VA Project/ML_RPA_Use_Cases/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="8_{A196FC46-37C7-497A-8168-3DF98752043B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F22F89CC-F6B1-4F35-822A-D32B41D5562C}"/>
+  <xr:revisionPtr revIDLastSave="268" documentId="8_{A196FC46-37C7-497A-8168-3DF98752043B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD8011F4-796F-48D5-8745-D97B8DCB6C94}"/>
   <bookViews>
-    <workbookView xWindow="-20970" yWindow="9345" windowWidth="17130" windowHeight="14625" xr2:uid="{3A809188-EDBE-4730-9950-7A0D0331F8B9}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{3A809188-EDBE-4730-9950-7A0D0331F8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Cancer" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Code</t>
   </si>
@@ -62,36 +62,78 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
     <t>INQ030</t>
   </si>
   <si>
     <t>Do You Get Income From Social Security?</t>
   </si>
   <si>
+    <t>Yes;No;Refused;Don't Know;Missing</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>KIQ005</t>
   </si>
   <si>
     <t>How Often Do You Have Urinary Leakage per week?</t>
   </si>
   <si>
+    <t>Never;Less than once a month;A few times a month;A few times a week; Ever day and/or night; Refused;Don't Know;Missing</t>
+  </si>
+  <si>
+    <t>Less than once a month</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>AUQ054</t>
   </si>
   <si>
     <t>General Condition of Hearing?</t>
   </si>
   <si>
+    <t>Excellent;Good;A little trouble;Moderate hearing trouble;A lot of trouble;Deaf;Refused;Don't Know;Missing</t>
+  </si>
+  <si>
+    <t>A little trouble</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>MCQ560</t>
   </si>
   <si>
     <t>Have You Ever Had GallBladder Surgery?</t>
   </si>
   <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>MCQ371D</t>
   </si>
   <si>
     <t>Are you watching your weight?</t>
   </si>
   <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>HUQ071</t>
   </si>
   <si>
@@ -104,12 +146,21 @@
     <t>Main Reason for Visiting Dentist?</t>
   </si>
   <si>
+    <t>Went in on own for check-up, examination, or cleaning;Was called in by dentist for check-up, examination, or cleaning;Something was wrong, bothering, or hurting; Went for treatment of a condition that dentist previously discovered;Other;Refused;Don't Know;Missing</t>
+  </si>
+  <si>
+    <t>Something was wrong, bothering, or hurting</t>
+  </si>
+  <si>
     <t>MCQ092</t>
   </si>
   <si>
     <t>Received Blood Transfusion?</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>SMQ020</t>
   </si>
   <si>
@@ -122,25 +173,19 @@
     <t>Over the Last Two Weeks have You Felt Tired or Had Little Energy?</t>
   </si>
   <si>
+    <t>Not at all;Several Days;More than half the days;Nearly every day;Refused;Don't Know;Missing</t>
+  </si>
+  <si>
+    <t>Several Days</t>
+  </si>
+  <si>
     <t>PUQ110</t>
   </si>
   <si>
     <t xml:space="preserve">Any Chemical Products Used to Kill Weeds? </t>
   </si>
   <si>
-    <t>Yes;No;Refused;Don't Know;Missing</t>
-  </si>
-  <si>
-    <t>Never;Less than once a month;A few times a month;A few times a week; Ever day and/or night; Refused;Don't Know;Missing</t>
-  </si>
-  <si>
-    <t>Excellent;Good;A little trouble;Moderate hearing trouble;A lot of trouble;Deaf;Refused;Don't Know;Missing</t>
-  </si>
-  <si>
-    <t>Went in on own for check-up, examination, or cleaning;Was called in by dentist for check-up, examination, or cleaning;Something was wrong, bothering, or hurting; Went for treatment of a condition that dentist previously discovered;Other;Refused;Don't Know;Missing</t>
-  </si>
-  <si>
-    <t>Not at all;Several Days;More than half the days;Nearly every day;Refused;Don't Know;Missing</t>
+    <t>Refused</t>
   </si>
 </sst>
 </file>
@@ -188,7 +233,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -223,13 +273,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Test_ML_RPA_File" displayName="Test_ML_RPA_File" ref="A1:D12" totalsRowShown="0">
-  <autoFilter ref="A1:D12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Code" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Question" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Answer Options" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Answer" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Test_ML_RPA_File" displayName="Test_ML_RPA_File" ref="A1:E12" totalsRowShown="0">
+  <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Code" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Question" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Answer Options" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Answer" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Coefficient" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -532,21 +583,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56D7271-7352-4CE3-9491-49EDC88F3678}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="234.31640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6796875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="221.04296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,126 +611,195 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>